<commit_message>
added parameeter to INTERPOLATE function to control behaviour with label output
</commit_message>
<xml_diff>
--- a/UsefulFunctions_demo.xlsx
+++ b/UsefulFunctions_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\UsefulFunctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9DDB2-AAD7-45DF-87D1-8576FB0C53B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30D603-612C-4E4A-ADA7-26D13B30E9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{39B80353-6C67-49F1-9EE2-84E64DE65129}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>A</t>
   </si>
@@ -166,9 +166,6 @@
     <t>extrapolating</t>
   </si>
   <si>
-    <t>=Interpolate()</t>
-  </si>
-  <si>
     <t>=DaysOfMonth()</t>
   </si>
   <si>
@@ -245,6 +242,254 @@
   </si>
   <si>
     <t>racecar</t>
+  </si>
+  <si>
+    <r>
+      <t>=Interpolate()</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on numerical data</t>
+    </r>
+  </si>
+  <si>
+    <t>numbers</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>text_interpolation</t>
+  </si>
+  <si>
+    <t>if found, return the label at the position of the second argument in the numeric column</t>
+  </si>
+  <si>
+    <r>
+      <t>=Interpolate()</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on table with labels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">by default (or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) will return a message declaring the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> labels limiting the range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for the searched number.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as argument for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text_interpolation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will return the label</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> before</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the searched number.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as argument for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text_interpolation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will return the label</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> after</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the searched number.</t>
+    </r>
+  </si>
+  <si>
+    <t>will return a #NULL! Error when extrapolating on the label columns, if not posible to define a correct output</t>
   </si>
 </sst>
 </file>
@@ -252,9 +497,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +519,39 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -385,50 +663,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,9 +1794,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1559,7 +1834,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1665,7 +1940,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1807,7 +2082,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1816,10 +2091,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B17285B-73CD-42A4-958F-7D71CF75033A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Z1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1845,213 +2120,269 @@
     <col min="25" max="25" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="106.77734375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6.44140625" customWidth="1"/>
-    <col min="28" max="28" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21" customWidth="1"/>
-    <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="10.5546875" customWidth="1"/>
+    <col min="30" max="30" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="90.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.44140625" customWidth="1"/>
+    <col min="38" max="38" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21" customWidth="1"/>
+    <col min="44" max="44" width="13" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="19"/>
-      <c r="C1" s="5"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="19"/>
       <c r="G1" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="K1" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L1" s="18"/>
       <c r="N1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="18"/>
+      <c r="Q1" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM1" s="12"/>
+      <c r="AO1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP1" s="18"/>
+      <c r="AR1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS1" s="18"/>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="21"/>
+      <c r="AD2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="Q1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="25" t="s">
+      <c r="N3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="26"/>
-      <c r="AE1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" s="18"/>
-      <c r="AH1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" s="18"/>
-    </row>
-    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2074,52 +2405,69 @@
         <f t="array" ref="I4">[1]!daysOfMonth(G4)</f>
         <v>31</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="15">
         <v>0.85</v>
       </c>
-      <c r="L4" s="23" cm="1">
+      <c r="L4" s="14" cm="1">
         <f t="array" ref="L4">[1]!Density2Gradient(K4)</f>
         <v>0.36813509444444448</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="14">
         <v>0.33</v>
       </c>
-      <c r="O4" s="24" cm="1">
+      <c r="O4" s="15" cm="1">
         <f t="array" ref="O4">[1]!Gradient2Density(N4)</f>
         <v>0.76194854615342977</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AB4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC4" cm="1">
-        <f t="array" ref="AC4">[1]!NUMBERinTEXT(AB4)</f>
+      <c r="AB4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="26"/>
+      <c r="AI4" t="str" cm="1">
+        <f t="array" ref="AI4">[1]!INTERPOLATE($AB$5:$AC$10,AD4,AE4,AF4,AG4,AH4)</f>
+        <v>one</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM4" cm="1">
+        <f t="array" ref="AM4">[1]!NUMBERinTEXT(AL4)</f>
         <v>6</v>
       </c>
-      <c r="AF4" t="str" cm="1">
-        <f t="array" ref="AF4">[1]!pwd()</f>
+      <c r="AP4" t="str" cm="1">
+        <f t="array" ref="AP4">[1]!pwd()</f>
         <v>D:\git\UsefulFunctions</v>
       </c>
-      <c r="AH4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI4" s="2" t="str" cm="1">
-        <f t="array" ref="AI4">[1]!Reverse(AH4)</f>
+      <c r="AR4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS4" t="str" cm="1">
+        <f t="array" ref="AS4">[1]!Reverse(AR4)</f>
         <v>fedcba</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2132,7 +2480,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="str" cm="1">
-        <f t="array" ref="E5">[1]!NUMtoABC(B5)</f>
+        <f t="array" ref="E5">[1]!NUMtoABC(D5)</f>
         <v>E</v>
       </c>
       <c r="G5">
@@ -2142,32 +2490,32 @@
         <f t="array" ref="I5">[1]!daysOfMonth(G5)</f>
         <v>29</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="15">
         <v>1</v>
       </c>
-      <c r="L5" s="23" cm="1">
+      <c r="L5" s="14" cm="1">
         <f t="array" ref="L5">[1]!Density2Gradient(K5)</f>
         <v>0.43310011111111113</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="14">
         <v>0.433</v>
       </c>
-      <c r="O5" s="24" cm="1">
+      <c r="O5" s="15" cm="1">
         <f t="array" ref="O5">[1]!Gradient2Density(N5)</f>
         <v>0.99976884995283355</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>-3</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5">
         <f>Q5^3</f>
         <v>-27</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5">
         <f>Q5^2</f>
         <v>9</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="6">
         <f t="shared" ref="T5:T6" si="1">Q5</f>
         <v>-3</v>
       </c>
@@ -2181,29 +2529,48 @@
       <c r="Z5" t="s">
         <v>26</v>
       </c>
-      <c r="AB5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC5" cm="1">
-        <f t="array" ref="AC5">[1]!NUMBERinTEXT(AB5)</f>
+      <c r="AB5" s="24">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD5">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="str" cm="1">
+        <f t="array" ref="AI5">[1]!INTERPOLATE($AB$5:$AC$10,AD5,AE5,AF5,AG5,AH5)</f>
+        <v>between three and five</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM5" cm="1">
+        <f t="array" ref="AM5">[1]!NUMBERinTEXT(AL5)</f>
         <v>2025</v>
       </c>
-      <c r="AE5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF5" t="str" cm="1">
-        <f t="array" ref="AF5">[1]!pwd(AE5)</f>
+      <c r="AO5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP5" t="str" cm="1">
+        <f t="array" ref="AP5">[1]!pwd(AO5)</f>
         <v>True</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AR5" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="2" t="str" cm="1">
-        <f t="array" ref="AI5">[1]!Reverse(AH5)</f>
+      <c r="AS5" t="str" cm="1">
+        <f t="array" ref="AS5">[1]!Reverse(AR5)</f>
         <v>dlrow olleh</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2216,7 +2583,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="str" cm="1">
-        <f t="array" ref="E6">[1]!NUMtoABC(B6)</f>
+        <f t="array" ref="E6">[1]!NUMtoABC(D6)</f>
         <v>J</v>
       </c>
       <c r="G6">
@@ -2226,32 +2593,32 @@
         <f t="array" ref="I6">[1]!daysOfMonth(G6)</f>
         <v>31</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="15">
         <v>1.05</v>
       </c>
-      <c r="L6" s="23" cm="1">
+      <c r="L6" s="14" cm="1">
         <f t="array" ref="L6">[1]!Density2Gradient(K6)</f>
         <v>0.45475511666666674</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="14">
         <v>0.5</v>
       </c>
-      <c r="O6" s="24" cm="1">
+      <c r="O6" s="15" cm="1">
         <f t="array" ref="O6">[1]!Gradient2Density(N6)</f>
         <v>1.1544674941718633</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>-2</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6">
         <f t="shared" ref="R6:R18" si="2">Q6^3</f>
         <v>-8</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6">
         <f t="shared" ref="S6:S18" si="3">Q6^2</f>
         <v>4</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="6">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
@@ -2265,35 +2632,54 @@
         <v>2</v>
       </c>
       <c r="Y6" cm="1">
-        <f t="array" ref="Y6">[1]!INTERPOLATE($Q$5:$T$18,U6,V6,W6)</f>
+        <f t="array" ref="Y6">[1]!INTERPOLATE($Q$5:$T$18,U6)</f>
         <v>4.5</v>
       </c>
       <c r="Z6" t="s">
         <v>25</v>
       </c>
-      <c r="AB6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC6" cm="1">
-        <f t="array" ref="AC6">[1]!NUMBERinTEXT(AB6)</f>
+      <c r="AB6" s="24">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="26">
+        <v>-1</v>
+      </c>
+      <c r="AI6" t="str" cm="1">
+        <f t="array" ref="AI6">[1]!INTERPOLATE($AB$5:$AC$10,AD6,AE6,AF6,AG6,AH6)</f>
+        <v>three</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM6" cm="1">
+        <f t="array" ref="AM6">[1]!NUMBERinTEXT(AL6)</f>
         <v>1.08</v>
       </c>
-      <c r="AE6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF6" t="str" cm="1">
-        <f t="array" ref="AF6">[1]!pwd(AE6)</f>
+      <c r="AO6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP6" t="str" cm="1">
+        <f t="array" ref="AP6">[1]!pwd(AO6)</f>
         <v>False</v>
       </c>
-      <c r="AH6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI6" s="2" t="str" cm="1">
-        <f t="array" ref="AI6">[1]!Reverse(AH6)</f>
+      <c r="AR6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS6" t="str" cm="1">
+        <f t="array" ref="AS6">[1]!Reverse(AR6)</f>
         <v>racecar</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2306,7 +2692,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="str" cm="1">
-        <f t="array" ref="E7">[1]!NUMtoABC(B7)</f>
+        <f t="array" ref="E7">[1]!NUMtoABC(D7)</f>
         <v>X</v>
       </c>
       <c r="G7">
@@ -2316,18 +2702,18 @@
         <f t="array" ref="I7">[1]!daysOfMonth(G7)</f>
         <v>30</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>-1</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="6">
         <f>Q7</f>
         <v>-1</v>
       </c>
@@ -2338,21 +2724,40 @@
         <v>4</v>
       </c>
       <c r="Y7" cm="1">
-        <f t="array" ref="Y7">[1]!INTERPOLATE($Q$5:$T$18,U7,V7,W7)</f>
-        <v>1</v>
+        <f t="array" ref="Y7">[1]!INTERPOLATE($Q$5:$T$18,U7)</f>
+        <v>4.5</v>
       </c>
       <c r="Z7" t="s">
         <v>27</v>
       </c>
-      <c r="AB7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC7" cm="1">
-        <f t="array" ref="AC7">[1]!NUMBERinTEXT(AB7)</f>
+      <c r="AB7" s="24">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AH7" s="26">
+        <v>1</v>
+      </c>
+      <c r="AI7" t="str" cm="1">
+        <f t="array" ref="AI7">[1]!INTERPOLATE($AB$5:$AC$10,AD7,AE7,AF7,AG7,AH7)</f>
+        <v>five</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM7" cm="1">
+        <f t="array" ref="AM7">[1]!NUMBERinTEXT(AL7)</f>
         <v>-20</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2365,7 +2770,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="str" cm="1">
-        <f t="array" ref="E8">[1]!NUMtoABC(B8)</f>
+        <f t="array" ref="E8">[1]!NUMtoABC(D8)</f>
         <v>Z</v>
       </c>
       <c r="G8">
@@ -2375,18 +2780,18 @@
         <f t="array" ref="I8">[1]!daysOfMonth(G8)</f>
         <v>31</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>0</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="6">
         <f t="shared" ref="T8:T9" si="4">Q8</f>
         <v>0</v>
       </c>
@@ -2397,14 +2802,28 @@
         <v>4</v>
       </c>
       <c r="Y8" cm="1">
-        <f t="array" ref="Y8">[1]!INTERPOLATE($Q$5:$T$18,U8,V8,W8)</f>
-        <v>6.5</v>
+        <f t="array" ref="Y8">[1]!INTERPOLATE($Q$5:$T$18,U8)</f>
+        <v>4.5</v>
       </c>
       <c r="Z8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB8" s="24">
+        <v>5</v>
+      </c>
+      <c r="AC8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD8">
+        <v>-1</v>
+      </c>
+      <c r="AH8" s="26"/>
+      <c r="AI8" t="str" cm="1">
+        <f t="array" ref="AI8">[1]!INTERPOLATE($AB$5:$AC$10,AD8,AE8,AF8,AG8,AH8)</f>
+        <v>before one</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2417,7 +2836,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="str" cm="1">
-        <f t="array" ref="E9">[1]!NUMtoABC(B9)</f>
+        <f t="array" ref="E9">[1]!NUMtoABC(D9)</f>
         <v>AA</v>
       </c>
       <c r="G9">
@@ -2427,18 +2846,18 @@
         <f t="array" ref="I9">[1]!daysOfMonth(G9)</f>
         <v>30</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>1</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -2452,14 +2871,33 @@
         <v>1</v>
       </c>
       <c r="Y9" cm="1">
-        <f t="array" ref="Y9">[1]!INTERPOLATE($Q$5:$T$18,U9,V9,W9)</f>
-        <v>1.0714285714285714</v>
+        <f t="array" ref="Y9">[1]!INTERPOLATE($Q$5:$T$18,U9)</f>
+        <v>4.5</v>
       </c>
       <c r="Z9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB9" s="24">
+        <v>7</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD9">
+        <v>-1</v>
+      </c>
+      <c r="AH9" s="26">
+        <v>-1</v>
+      </c>
+      <c r="AI9" t="e" cm="1">
+        <f t="array" ref="AI9">[1]!INTERPOLATE($AB$5:$AC$10,AD9,AE9,AF9,AG9,AH9)</f>
+        <v>#NULL!</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2472,7 +2910,7 @@
         <v>633</v>
       </c>
       <c r="E10" t="str" cm="1">
-        <f t="array" ref="E10">[1]!NUMtoABC(B10)</f>
+        <f t="array" ref="E10">[1]!NUMtoABC(D10)</f>
         <v>XI</v>
       </c>
       <c r="G10">
@@ -2482,18 +2920,18 @@
         <f t="array" ref="I10">[1]!daysOfMonth(G10)</f>
         <v>31</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <v>2</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="6">
         <v>1</v>
       </c>
       <c r="U10">
@@ -2506,14 +2944,30 @@
         <v>2</v>
       </c>
       <c r="Y10" cm="1">
-        <f t="array" ref="Y10">[1]!INTERPOLATE($Q$5:$T$18,U10,V10,W10)</f>
-        <v>1.5</v>
+        <f t="array" ref="Y10">[1]!INTERPOLATE($Q$5:$T$18,U10)</f>
+        <v>4.5</v>
       </c>
       <c r="Z10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB10" s="25">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD10">
+        <v>-1</v>
+      </c>
+      <c r="AH10" s="26">
+        <v>1</v>
+      </c>
+      <c r="AI10" t="str" cm="1">
+        <f t="array" ref="AI10">[1]!INTERPOLATE($AB$5:$AC$10,AD10,AE10,AF10,AG10,AH10)</f>
+        <v>one</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2980,7 @@
         <v>3752127</v>
       </c>
       <c r="E11" t="str" cm="1">
-        <f t="array" ref="E11">[1]!NUMtoABC(B11)</f>
+        <f t="array" ref="E11">[1]!NUMtoABC(D11)</f>
         <v>HELLO</v>
       </c>
       <c r="G11">
@@ -2536,18 +2990,18 @@
         <f t="array" ref="I11">[1]!daysOfMonth(G11)</f>
         <v>31</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>3</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="6">
         <f>T10+T9</f>
         <v>2</v>
       </c>
@@ -2558,14 +3012,22 @@
         <v>3</v>
       </c>
       <c r="Y11" cm="1">
-        <f t="array" ref="Y11">[1]!INTERPOLATE($Q$5:$T$18,U11,V11,W11)</f>
-        <v>-1.5</v>
+        <f t="array" ref="Y11">[1]!INTERPOLATE($Q$5:$T$18,U11)</f>
+        <v>4.5</v>
       </c>
       <c r="Z11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AD11">
+        <v>11</v>
+      </c>
+      <c r="AH11" s="26"/>
+      <c r="AI11" t="str" cm="1">
+        <f t="array" ref="AI11">[1]!INTERPOLATE($AB$5:$AC$10,AD11,AE11,AF11,AG11,AH11)</f>
+        <v>after ten</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2578,7 +3040,7 @@
         <v>10786572</v>
       </c>
       <c r="E12" t="str" cm="1">
-        <f t="array" ref="E12">[1]!NUMtoABC(B12)</f>
+        <f t="array" ref="E12">[1]!NUMtoABC(D12)</f>
         <v>WORLD</v>
       </c>
       <c r="G12">
@@ -2588,18 +3050,18 @@
         <f t="array" ref="I12">[1]!daysOfMonth(G12)</f>
         <v>30</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="5">
         <v>4</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="6">
         <f t="shared" ref="T12:T18" si="5">T11+T10</f>
         <v>3</v>
       </c>
@@ -2607,20 +3069,30 @@
         <v>15</v>
       </c>
       <c r="Y12" cm="1">
-        <f t="array" ref="Y12">[1]!INTERPOLATE($Q$5:$T$18,U12,V12,W12)</f>
+        <f t="array" ref="Y12">[1]!INTERPOLATE($Q$5:$T$18,U12)</f>
         <v>2355</v>
       </c>
       <c r="Z12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AD12">
+        <v>11</v>
+      </c>
+      <c r="AH12" s="26">
+        <v>-1</v>
+      </c>
+      <c r="AI12" t="str" cm="1">
+        <f t="array" ref="AI12">[1]!INTERPOLATE($AB$5:$AC$10,AD12,AE12,AF12,AG12,AH12)</f>
+        <v>seven</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="D13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" t="str" cm="1">
-        <f t="array" ref="E13">[1]!NUMtoABC(B13)</f>
+        <f t="array" ref="E13">[1]!NUMtoABC(D13)</f>
         <v/>
       </c>
       <c r="G13">
@@ -2630,14 +3102,14 @@
         <f t="array" ref="I13">[1]!daysOfMonth(G13)</f>
         <v>31</v>
       </c>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="8">
+      <c r="Q13" s="5"/>
+      <c r="R13">
         <v>125</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13">
         <v>25</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="6">
         <f>T12+T11</f>
         <v>5</v>
       </c>
@@ -2645,14 +3117,24 @@
         <v>-4</v>
       </c>
       <c r="Y13" cm="1">
-        <f t="array" ref="Y13">[1]!INTERPOLATE($Q$5:$T$18,U13,V13,W13)</f>
+        <f t="array" ref="Y13">[1]!INTERPOLATE($Q$5:$T$18,U13)</f>
         <v>-46</v>
       </c>
       <c r="Z13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AD13">
+        <v>11</v>
+      </c>
+      <c r="AH13" s="26">
+        <v>1</v>
+      </c>
+      <c r="AI13" t="e" cm="1">
+        <f t="array" ref="AI13">[1]!INTERPOLATE($AB$5:$AC$10,AD13,AE13,AF13,AG13,AH13)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G14">
         <v>11</v>
       </c>
@@ -2660,18 +3142,18 @@
         <f t="array" ref="I14">[1]!daysOfMonth(G14)</f>
         <v>30</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="5">
         <v>6</v>
       </c>
-      <c r="R14" s="8">
+      <c r="R14">
         <f t="shared" si="2"/>
         <v>216</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S14">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="6">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -2679,17 +3161,17 @@
         <v>1.5</v>
       </c>
       <c r="X14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y14" cm="1">
+        <f t="array" ref="Y14">[1]!INTERPOLATE($Q$5:$T$18,U14)</f>
+        <v>4.5</v>
+      </c>
+      <c r="Z14" t="s">
         <v>53</v>
       </c>
-      <c r="Y14" cm="1">
-        <f t="array" ref="Y14">[1]!INTERPOLATE($Q$5:$T$18,U14,V14,W14,X14)</f>
-        <v>4.5</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G15">
         <v>12</v>
       </c>
@@ -2697,18 +3179,18 @@
         <f t="array" ref="I15">[1]!daysOfMonth(G15)</f>
         <v>31</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="5">
         <v>7</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15">
         <f t="shared" si="2"/>
         <v>343</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="6">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
@@ -2716,14 +3198,14 @@
         <v>1.5</v>
       </c>
       <c r="Y15" cm="1">
-        <f t="array" ref="Y15">[1]!INTERPOLATE(another_sheet!$Q$5:$T$18,U15,V15,W15,X15)</f>
+        <f t="array" ref="Y15">[1]!INTERPOLATE($Q$5:$T$18,U15)</f>
         <v>4.5</v>
       </c>
       <c r="Z15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G16" s="1">
         <v>45337</v>
       </c>
@@ -2732,18 +3214,18 @@
         <f t="array" ref="I16">[1]!daysOfMonth(G16)</f>
         <v>29</v>
       </c>
-      <c r="Q16" s="27">
+      <c r="Q16" s="5">
         <v>8</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="S16" s="28">
+      <c r="S16">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="6">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
@@ -2757,11 +3239,11 @@
         <v>4</v>
       </c>
       <c r="Y16" cm="1">
-        <f t="array" ref="Y16">[1]!INTERPOLATE($Q$5:$T$18,U16,V16,W16,X16)</f>
-        <v>7.5</v>
+        <f t="array" ref="Y16">[1]!INTERPOLATE($Q$5:$T$18,U16)</f>
+        <v>200.83333333333334</v>
       </c>
       <c r="Z16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="7:26" x14ac:dyDescent="0.3">
@@ -2773,15 +3255,14 @@
         <f t="array" ref="I17">[1]!daysOfMonth(G17)</f>
         <v>28</v>
       </c>
-      <c r="Q17" s="27">
+      <c r="Q17" s="5">
         <v>9</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17">
         <f t="shared" si="2"/>
         <v>729</v>
       </c>
-      <c r="S17" s="28"/>
-      <c r="T17" s="9">
+      <c r="T17" s="6">
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
@@ -2795,11 +3276,11 @@
         <v>3</v>
       </c>
       <c r="Y17" cm="1">
-        <f t="array" ref="Y17">[1]!INTERPOLATE($Q$5:$T$18,U17,V17,W17,X17)</f>
-        <v>82</v>
+        <f t="array" ref="Y17">[1]!INTERPOLATE($Q$5:$T$18,U17)</f>
+        <v>729</v>
       </c>
       <c r="Z17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="7:26" x14ac:dyDescent="0.3">
@@ -2810,18 +3291,18 @@
         <f t="array" ref="I18">[1]!daysOfMonth(G18)</f>
         <v>30.416666030883789</v>
       </c>
-      <c r="Q18" s="29">
+      <c r="Q18" s="16">
         <v>10</v>
       </c>
-      <c r="R18" s="30">
+      <c r="R18" s="17">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="S18" s="30">
+      <c r="S18" s="17">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="T18" s="10">
+      <c r="T18" s="7">
         <f t="shared" si="5"/>
         <v>55</v>
       </c>
@@ -2843,8 +3324,8 @@
         <v>2023</v>
       </c>
       <c r="I20" cm="1">
-        <f t="array" ref="I20">[1]!daysOfMonth(G20, H20)</f>
-        <v>28</v>
+        <f t="array" ref="I20">[1]!daysOfMonth(G20)</f>
+        <v>29</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -2865,7 +3346,7 @@
         <v>2024</v>
       </c>
       <c r="I21" cm="1">
-        <f t="array" ref="I21">[1]!daysOfMonth(G21, H21)</f>
+        <f t="array" ref="I21">[1]!daysOfMonth(G21)</f>
         <v>29</v>
       </c>
       <c r="U21">
@@ -2950,17 +3431,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="13">
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB1:AJ1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="Q1:Z1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2979,268 +3463,268 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
     </row>
     <row r="3" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
     </row>
     <row r="4" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>-3</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5">
         <f>Q5^3</f>
         <v>-27</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5">
         <f>Q5^2</f>
         <v>9</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="6">
         <f t="shared" ref="T5:T6" si="0">Q5</f>
         <v>-3</v>
       </c>
     </row>
     <row r="6" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>-2</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6">
         <f t="shared" ref="R6:R18" si="1">Q6^3</f>
         <v>-8</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6">
         <f t="shared" ref="S6:S18" si="2">Q6^2</f>
         <v>4</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="6">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
     </row>
     <row r="7" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>-1</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="6">
         <f>Q7</f>
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>0</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="6">
         <f t="shared" ref="T8:T9" si="3">Q8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>1</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S9" s="8">
+      <c r="S9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <v>2</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>3</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="6">
         <f>T10+T9</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q12" s="6">
+      <c r="Q12" s="5">
         <v>4</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="6">
         <f t="shared" ref="T12:T18" si="4">T11+T10</f>
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>5</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13">
         <f t="shared" ref="S13" si="5">Q13^2</f>
         <v>25</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="6">
         <f>T12+T11</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q14" s="6">
+      <c r="Q14" s="5">
         <v>6</v>
       </c>
-      <c r="R14" s="8">
+      <c r="R14">
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S14">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="6">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q15" s="6">
+      <c r="Q15" s="5">
         <v>7</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15">
         <f t="shared" si="1"/>
         <v>343</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="6">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q16" s="27">
+      <c r="Q16" s="5">
         <v>8</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16">
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-      <c r="S16" s="28">
+      <c r="S16">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="6">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q17" s="27">
+      <c r="Q17" s="5">
         <v>9</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17">
         <f t="shared" si="1"/>
         <v>729</v>
       </c>
-      <c r="S17" s="28">
+      <c r="S17">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="6">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="17:20" x14ac:dyDescent="0.3">
-      <c r="Q18" s="29">
+      <c r="Q18" s="16">
         <v>10</v>
       </c>
-      <c r="R18" s="30">
+      <c r="R18" s="17">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="S18" s="30">
+      <c r="S18" s="17">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="T18" s="10">
+      <c r="T18" s="7">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>

</xml_diff>